<commit_message>
Issue with empty time and needs to collect stats
</commit_message>
<xml_diff>
--- a/Projekt/ArrivalProfiles.xlsx
+++ b/Projekt/ArrivalProfiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s204617_dtu_dk/Documents/Decisions under uncertainty/Projekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A608C0F-55A4-4525-AA90-B2AB220F4F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{3A608C0F-55A4-4525-AA90-B2AB220F4F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E614BCD-888C-43A5-9CD0-7DF968860B8A}"/>
   <bookViews>
-    <workbookView xWindow="2090" yWindow="3220" windowWidth="29600" windowHeight="14260" xr2:uid="{D3509A2E-A134-450D-BC36-7D71AE3656B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D3509A2E-A134-450D-BC36-7D71AE3656B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>expected arrivals per hour</t>
   </si>
@@ -43,35 +43,26 @@
     <t>Nørreport--DTU</t>
   </si>
   <si>
-    <t>0.1</t>
-  </si>
-  <si>
     <t>DTU--Nørreport</t>
   </si>
   <si>
     <t>expected travel time in hours</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.55</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>0.65</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,10 +407,13 @@
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AA8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -506,23 +500,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>SUM(C2:AA2)</f>
         <v>275</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>0.1</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -569,14 +562,14 @@
       <c r="V2">
         <v>5</v>
       </c>
-      <c r="W2" t="s">
-        <v>2</v>
-      </c>
-      <c r="X2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>2</v>
+      <c r="W2">
+        <v>0.1</v>
+      </c>
+      <c r="X2">
+        <v>0.1</v>
+      </c>
+      <c r="Y2">
+        <v>0.1</v>
       </c>
       <c r="Z2">
         <v>10</v>
@@ -587,29 +580,28 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <f>SUM(C3:AA3)</f>
         <v>275</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>2</v>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3">
+        <v>0.1</v>
+      </c>
+      <c r="H3">
+        <v>0.1</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -665,176 +657,177 @@
       <c r="Z3">
         <v>5</v>
       </c>
-      <c r="AA3" t="s">
-        <v>2</v>
+      <c r="AA3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" t="s">
-        <v>5</v>
-      </c>
-      <c r="N7" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" t="s">
-        <v>5</v>
-      </c>
-      <c r="P7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R7" t="s">
-        <v>6</v>
-      </c>
-      <c r="S7" t="s">
-        <v>7</v>
-      </c>
-      <c r="T7" t="s">
-        <v>8</v>
-      </c>
-      <c r="U7" t="s">
-        <v>7</v>
-      </c>
-      <c r="V7" t="s">
-        <v>5</v>
-      </c>
-      <c r="W7" t="s">
-        <v>5</v>
-      </c>
-      <c r="X7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>5</v>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M7">
+        <v>0.5</v>
+      </c>
+      <c r="N7">
+        <v>0.5</v>
+      </c>
+      <c r="O7">
+        <v>0.5</v>
+      </c>
+      <c r="P7">
+        <v>0.5</v>
+      </c>
+      <c r="Q7">
+        <v>0.5</v>
+      </c>
+      <c r="R7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S7">
+        <v>0.6</v>
+      </c>
+      <c r="T7">
+        <v>0.65</v>
+      </c>
+      <c r="U7">
+        <v>0.6</v>
+      </c>
+      <c r="V7">
+        <v>0.5</v>
+      </c>
+      <c r="W7">
+        <v>0.5</v>
+      </c>
+      <c r="X7">
+        <v>0.5</v>
+      </c>
+      <c r="Y7">
+        <v>0.5</v>
+      </c>
+      <c r="Z7">
+        <v>0.5</v>
+      </c>
+      <c r="AA7">
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N8" t="s">
-        <v>5</v>
-      </c>
-      <c r="O8" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>5</v>
-      </c>
-      <c r="R8" t="s">
-        <v>6</v>
-      </c>
-      <c r="S8" t="s">
-        <v>6</v>
-      </c>
-      <c r="T8" t="s">
-        <v>6</v>
-      </c>
-      <c r="U8" t="s">
-        <v>6</v>
-      </c>
-      <c r="V8" t="s">
-        <v>5</v>
-      </c>
-      <c r="W8" t="s">
-        <v>5</v>
-      </c>
-      <c r="X8" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
+        <v>0.5</v>
+      </c>
+      <c r="I8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J8">
+        <v>0.6</v>
+      </c>
+      <c r="K8">
+        <v>0.6</v>
+      </c>
+      <c r="L8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M8">
+        <v>0.5</v>
+      </c>
+      <c r="N8">
+        <v>0.5</v>
+      </c>
+      <c r="O8">
+        <v>0.5</v>
+      </c>
+      <c r="P8">
+        <v>0.5</v>
+      </c>
+      <c r="Q8">
+        <v>0.5</v>
+      </c>
+      <c r="R8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="U8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="V8">
+        <v>0.5</v>
+      </c>
+      <c r="W8">
+        <v>0.5</v>
+      </c>
+      <c r="X8">
+        <v>0.5</v>
+      </c>
+      <c r="Y8">
+        <v>0.5</v>
+      </c>
+      <c r="Z8">
+        <v>0.5</v>
+      </c>
+      <c r="AA8">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
24/04/2022 - Rebalance still not working
</commit_message>
<xml_diff>
--- a/Projekt/ArrivalProfiles.xlsx
+++ b/Projekt/ArrivalProfiles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s204617_dtu_dk/Documents/Decisions under uncertainty/Projekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{3A608C0F-55A4-4525-AA90-B2AB220F4F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E614BCD-888C-43A5-9CD0-7DF968860B8A}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{3A608C0F-55A4-4525-AA90-B2AB220F4F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D0CC0B0-6063-4A57-AC6C-66FFC564E305}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D3509A2E-A134-450D-BC36-7D71AE3656B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D3509A2E-A134-450D-BC36-7D71AE3656B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0996C00-2215-4A0B-BECA-F6EE9E76938E}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>